<commit_message>
feat: convert May-Aug in 2022
</commit_message>
<xml_diff>
--- a/22年力扣每日一题做题情况.xlsx
+++ b/22年力扣每日一题做题情况.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6653C2E7-5A59-4522-92E3-EE981356058A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF0ED2A-2502-4D43-9C9C-0C5F2EE29A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="16155" windowHeight="8505" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="22年1月" sheetId="2" r:id="rId1"/>
@@ -25,6 +25,17 @@
     <sheet name="竞赛模板" sheetId="9" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -4827,7 +4838,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4886,6 +4897,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -21850,34 +21864,34 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="30" t="s">
         <v>293</v>
       </c>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
     </row>
     <row r="44" spans="1:5" ht="57.6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
@@ -21886,32 +21900,32 @@
       <c r="A46" s="1"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
+      <c r="A47" s="31"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="30"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
+      <c r="A48" s="31"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="30"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
+      <c r="A49" s="31"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="30"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
+      <c r="A50" s="31"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="1"/>
@@ -22742,32 +22756,32 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="14"/>
@@ -23585,34 +23599,34 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="29"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="15"/>
@@ -23715,7 +23729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53503CBA-3042-452B-9B01-B94B07C13766}">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -25467,39 +25481,39 @@
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -25527,8 +25541,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -26208,18 +26222,18 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="31"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
+      <c r="A41" s="32"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
     </row>
     <row r="42" spans="1:5" ht="57.6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="31"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
+      <c r="A42" s="32"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
@@ -26341,8 +26355,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -27213,8 +27227,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -27256,7 +27270,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="7">
-        <v>44287</v>
+        <v>44652</v>
       </c>
       <c r="B2">
         <v>954</v>
@@ -27275,8 +27289,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="7">
-        <v>44288</v>
+      <c r="A3" s="29">
+        <v>44653</v>
       </c>
       <c r="B3">
         <v>420</v>
@@ -27295,8 +27309,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" s="7">
-        <v>44289</v>
+      <c r="A4" s="29">
+        <v>44654</v>
       </c>
       <c r="B4">
         <v>744</v>
@@ -27315,8 +27329,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="7">
-        <v>44290</v>
+      <c r="A5" s="29">
+        <v>44655</v>
       </c>
       <c r="B5">
         <v>307</v>
@@ -27341,8 +27355,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" s="7">
-        <v>44291</v>
+      <c r="A6" s="29">
+        <v>44656</v>
       </c>
       <c r="B6">
         <v>762</v>
@@ -27364,8 +27378,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" s="7">
-        <v>44292</v>
+      <c r="A7" s="29">
+        <v>44657</v>
       </c>
       <c r="B7">
         <v>310</v>
@@ -27387,8 +27401,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="7">
-        <v>44293</v>
+      <c r="A8" s="29">
+        <v>44658</v>
       </c>
       <c r="B8">
         <v>796</v>
@@ -27410,8 +27424,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="7">
-        <v>44294</v>
+      <c r="A9" s="29">
+        <v>44659</v>
       </c>
       <c r="B9">
         <v>429</v>
@@ -27430,8 +27444,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="7">
-        <v>44295</v>
+      <c r="A10" s="29">
+        <v>44660</v>
       </c>
       <c r="B10">
         <v>780</v>
@@ -27450,8 +27464,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="7">
-        <v>44296</v>
+      <c r="A11" s="29">
+        <v>44661</v>
       </c>
       <c r="B11">
         <v>804</v>
@@ -27470,8 +27484,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="7">
-        <v>44297</v>
+      <c r="A12" s="29">
+        <v>44662</v>
       </c>
       <c r="B12">
         <v>357</v>
@@ -27490,8 +27504,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="7">
-        <v>44298</v>
+      <c r="A13" s="29">
+        <v>44663</v>
       </c>
       <c r="B13">
         <v>806</v>
@@ -27510,8 +27524,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="7">
-        <v>44299</v>
+      <c r="A14" s="29">
+        <v>44664</v>
       </c>
       <c r="B14">
         <v>380</v>
@@ -27533,8 +27547,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="7">
-        <v>44300</v>
+      <c r="A15" s="29">
+        <v>44665</v>
       </c>
       <c r="B15">
         <v>1672</v>
@@ -27556,8 +27570,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="7">
-        <v>44301</v>
+      <c r="A16" s="29">
+        <v>44666</v>
       </c>
       <c r="B16">
         <v>385</v>
@@ -27576,8 +27590,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="7">
-        <v>44302</v>
+      <c r="A17" s="29">
+        <v>44667</v>
       </c>
       <c r="B17">
         <v>479</v>
@@ -27599,8 +27613,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="7">
-        <v>44303</v>
+      <c r="A18" s="29">
+        <v>44668</v>
       </c>
       <c r="B18">
         <v>819</v>
@@ -27622,8 +27636,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="7">
-        <v>44304</v>
+      <c r="A19" s="29">
+        <v>44669</v>
       </c>
       <c r="B19">
         <v>386</v>
@@ -27645,8 +27659,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="7">
-        <v>44305</v>
+      <c r="A20" s="29">
+        <v>44670</v>
       </c>
       <c r="B20">
         <v>821</v>
@@ -27665,8 +27679,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="7">
-        <v>44306</v>
+      <c r="A21" s="29">
+        <v>44671</v>
       </c>
       <c r="B21">
         <v>388</v>
@@ -27685,8 +27699,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A22" s="7">
-        <v>44307</v>
+      <c r="A22" s="29">
+        <v>44672</v>
       </c>
       <c r="B22">
         <v>824</v>
@@ -27705,8 +27719,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A23" s="7">
-        <v>44308</v>
+      <c r="A23" s="29">
+        <v>44673</v>
       </c>
       <c r="B23">
         <v>396</v>
@@ -27725,8 +27739,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A24" s="7">
-        <v>44309</v>
+      <c r="A24" s="29">
+        <v>44674</v>
       </c>
       <c r="B24">
         <v>587</v>
@@ -27748,8 +27762,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A25" s="7">
-        <v>44310</v>
+      <c r="A25" s="29">
+        <v>44675</v>
       </c>
       <c r="B25">
         <v>868</v>
@@ -27768,8 +27782,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A26" s="7">
-        <v>44311</v>
+      <c r="A26" s="29">
+        <v>44676</v>
       </c>
       <c r="B26">
         <v>398</v>
@@ -27791,8 +27805,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A27" s="7">
-        <v>44312</v>
+      <c r="A27" s="29">
+        <v>44677</v>
       </c>
       <c r="B27">
         <v>883</v>
@@ -27811,8 +27825,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="7">
-        <v>44313</v>
+      <c r="A28" s="29">
+        <v>44678</v>
       </c>
       <c r="B28">
         <v>417</v>
@@ -27834,8 +27848,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A29" s="7">
-        <v>44314</v>
+      <c r="A29" s="29">
+        <v>44679</v>
       </c>
       <c r="B29">
         <v>905</v>
@@ -27854,8 +27868,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" s="7">
-        <v>44315</v>
+      <c r="A30" s="29">
+        <v>44680</v>
       </c>
       <c r="B30">
         <v>427</v>
@@ -27874,8 +27888,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A31" s="7">
-        <v>44316</v>
+      <c r="A31" s="29">
+        <v>44681</v>
       </c>
       <c r="B31">
         <v>908</v>
@@ -28090,7 +28104,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
@@ -28869,27 +28883,27 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="29" t="s">
+      <c r="A43" s="30" t="s">
         <v>783</v>
       </c>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="8"/>
@@ -29739,25 +29753,25 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
@@ -30616,41 +30630,41 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="29" t="s">
+      <c r="A43" s="30" t="s">
         <v>848</v>
       </c>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="29"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="10"/>
@@ -31480,32 +31494,32 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="12"/>
@@ -32348,32 +32362,32 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="13"/>

</xml_diff>